<commit_message>
Added grey to the publishers
</commit_message>
<xml_diff>
--- a/data/data-extracted.xlsx
+++ b/data/data-extracted.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\replication-packages\twin-transition-survey-replication-package\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6708110C-D687-4FBD-B791-85EC14A7983C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0A1352-19B2-4AF5-8CD6-E99503EBBB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="420">
   <si>
     <t>Key</t>
   </si>
@@ -1729,6 +1729,9 @@
   </si>
   <si>
     <t>Undip</t>
+  </si>
+  <si>
+    <t>(Gray)</t>
   </si>
 </sst>
 </file>
@@ -2181,10 +2184,10 @@
   <dimension ref="A1:AF957"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2469,7 +2472,9 @@
       <c r="Z3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="AA3" s="11"/>
+      <c r="AA3" s="11" t="s">
+        <v>419</v>
+      </c>
       <c r="AB3" s="12">
         <v>2023</v>
       </c>
@@ -2725,6 +2730,9 @@
       </c>
       <c r="Z6" s="11" t="s">
         <v>126</v>
+      </c>
+      <c r="AA6" s="11" t="s">
+        <v>419</v>
       </c>
       <c r="AB6" s="12">
         <v>2023</v>
@@ -3666,6 +3674,9 @@
       <c r="Z17" s="11" t="s">
         <v>73</v>
       </c>
+      <c r="AA17" s="11" t="s">
+        <v>419</v>
+      </c>
       <c r="AB17" s="12">
         <v>2023</v>
       </c>
@@ -3830,6 +3841,9 @@
       </c>
       <c r="Z19" s="11" t="s">
         <v>326</v>
+      </c>
+      <c r="AA19" s="11" t="s">
+        <v>419</v>
       </c>
       <c r="AB19" s="12">
         <v>2024</v>

</xml_diff>